<commit_message>
Upload Files and manual UI enhancements
</commit_message>
<xml_diff>
--- a/Output.xlsx
+++ b/Output.xlsx
@@ -1,47 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kvp\Desktop\GL-Recon-App\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985E4635-E116-47B2-8562-81C6DB02275A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="$#,##0.00"/>
+  </numFmts>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -56,43 +48,95 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -380,22 +424,431 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F10001"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Comparison Key</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Original PO Amt (First)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Original PO Amount (Second)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Difference</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Dollar Difference</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Percentage Difference</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Acme Industrial Supply</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>529.15</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>-529.15</v>
+      </c>
+      <c r="F2" s="3" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Blue Ridge Packaging</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>42834.6</v>
+      </c>
+      <c r="C3" t="n">
+        <v>37063.48</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>5771.119999999995</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>0.1347303348227833</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Cedar Creek Electronics</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>10937.02</v>
+      </c>
+      <c r="C4" t="n">
+        <v>10985.77</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>-48.75</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>0.004457338470625453</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Delta Office Products</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>29001.86</v>
+      </c>
+      <c r="C5" t="n">
+        <v>27370.18</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>1631.68</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>0.05626121910801584</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Evergreen Safety Co.</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>2903.75</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>-2903.75</v>
+      </c>
+      <c r="F6" s="3" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Fulton Freight &amp; Logistics</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>11273.65</v>
+      </c>
+      <c r="C7" t="n">
+        <v>15584.36</v>
+      </c>
+      <c r="D7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>-4310.710000000001</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>0.3823703946814032</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Horizon IT Services</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4861.25</v>
+      </c>
+      <c r="C8" t="n">
+        <v>4861.25</v>
+      </c>
+      <c r="D8" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Ironclad Fasteners</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>12784.15</v>
+      </c>
+      <c r="C9" t="n">
+        <v>12672.76</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>111.3899999999994</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>0.008713133059296036</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Juniper Medical Supplies</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>8994.6</v>
+      </c>
+      <c r="C10" t="n">
+        <v>5048.440000000001</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>3946.16</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>0.4387254574967202</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Keystone Chemicals</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>16216.64</v>
+      </c>
+      <c r="C11" t="n">
+        <v>17118.14</v>
+      </c>
+      <c r="D11" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>-901.5</v>
+      </c>
+      <c r="F11" s="3" t="n">
+        <v>0.05559104722063263</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Lakeside Catering</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>14766.5</v>
+      </c>
+      <c r="C12" t="n">
+        <v>10503.83</v>
+      </c>
+      <c r="D12" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>4262.67</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>0.2886716554362916</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Metro Mechanical</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>1422.65</v>
+      </c>
+      <c r="D13" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>-1422.65</v>
+      </c>
+      <c r="F13" s="3" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Northstar Paper</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>15839.82</v>
+      </c>
+      <c r="C14" t="n">
+        <v>15742.14</v>
+      </c>
+      <c r="D14" t="b">
+        <v>1</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>97.68000000000029</v>
+      </c>
+      <c r="F14" s="3" t="n">
+        <v>0.006166736743220586</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Orion Plastics</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>3202.3</v>
+      </c>
+      <c r="C15" t="n">
+        <v>3202.32</v>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>-0.01999999999998181</v>
+      </c>
+      <c r="F15" s="3" t="n">
+        <v>6.245511038935081e-06</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Pinnacle Printing</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>8017.490000000001</v>
+      </c>
+      <c r="C16" t="n">
+        <v>13492.12</v>
+      </c>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>-5474.629999999998</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>0.682835900013595</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Riverbend Tools</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>11966.62</v>
+      </c>
+      <c r="C17" t="n">
+        <v>11988.05</v>
+      </c>
+      <c r="D17" t="b">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>-21.42999999999847</v>
+      </c>
+      <c r="F17" s="3" t="n">
+        <v>0.001790814783121589</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Summit Signage</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>5981.77</v>
+      </c>
+      <c r="C18" t="n">
+        <v>5984.06</v>
+      </c>
+      <c r="D18" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>-2.289999999999964</v>
+      </c>
+      <c r="F18" s="3" t="n">
+        <v>0.0003828298313041062</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Titan Textiles</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>2383.39</v>
+      </c>
+      <c r="C19" t="n">
+        <v>2395.21</v>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2" t="n">
+        <v>-11.82000000000016</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>0.004959322645475631</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>